<commit_message>
ajuste de dados de 2016 e inserção de dados BR
</commit_message>
<xml_diff>
--- a/dados/Excel/Eixo3_EstudaTrabalha.xlsx
+++ b/dados/Excel/Eixo3_EstudaTrabalha.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rebeca\Documents\Ibict\cotec-indicadores\dados\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bcasa\Ibict\cotec-indicadores\visao-2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14205" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14196" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="2019" sheetId="9" r:id="rId1"/>
@@ -22,6 +22,9 @@
     <sheet name="2012" sheetId="7" r:id="rId8"/>
     <sheet name="2011" sheetId="8" r:id="rId9"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId10"/>
+  </externalReferences>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -595,44 +598,44 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="39">
-    <cellStyle name="Hiperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -646,6 +649,41 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Dicionário da Planilha"/>
+      <sheetName val="Eixo 2"/>
+      <sheetName val="Eixo 3 - Série Histórica"/>
+      <sheetName val="Eixo 1"/>
+      <sheetName val="Eixo 3"/>
+      <sheetName val="Eixo 4"/>
+      <sheetName val="Eixo 5"/>
+      <sheetName val="Eixo 6 e 7"/>
+      <sheetName val="Eixo 8"/>
+      <sheetName val="Eixo 9"/>
+      <sheetName val="Eixo 10"/>
+      <sheetName val="Outros"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -976,22 +1014,22 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="16.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.69921875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.19921875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.125" customWidth="1"/>
+    <col min="11" max="11" width="13.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>55</v>
       </c>
@@ -1026,7 +1064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>43</v>
       </c>
@@ -1061,7 +1099,7 @@
         <v>255286</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="32" t="s">
         <v>1</v>
       </c>
@@ -1096,7 +1134,7 @@
         <v>107764</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="32" t="s">
         <v>7</v>
       </c>
@@ -1131,7 +1169,7 @@
         <v>596866</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="32" t="s">
         <v>45</v>
       </c>
@@ -1166,7 +1204,7 @@
         <v>83107</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="32" t="s">
         <v>27</v>
       </c>
@@ -1201,7 +1239,7 @@
         <v>1076035</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="32" t="s">
         <v>7</v>
       </c>
@@ -1236,7 +1274,7 @@
         <v>124459</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="32" t="s">
         <v>53</v>
       </c>
@@ -1271,7 +1309,7 @@
         <v>205498</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="32" t="s">
         <v>19</v>
       </c>
@@ -1306,7 +1344,7 @@
         <v>809146</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="32" t="s">
         <v>35</v>
       </c>
@@ -1341,7 +1379,7 @@
         <v>407634</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="32" t="s">
         <v>11</v>
       </c>
@@ -1376,7 +1414,7 @@
         <v>1185543</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="32" t="s">
         <v>39</v>
       </c>
@@ -1411,7 +1449,7 @@
         <v>412143</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="32" t="s">
         <v>29</v>
       </c>
@@ -1446,7 +1484,7 @@
         <v>449642</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="32" t="s">
         <v>33</v>
       </c>
@@ -1481,7 +1519,7 @@
         <v>1225384</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="32" t="s">
         <v>3</v>
       </c>
@@ -1516,7 +1554,7 @@
         <v>343017</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="32" t="s">
         <v>51</v>
       </c>
@@ -1551,7 +1589,7 @@
         <v>303323</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="32" t="s">
         <v>9</v>
       </c>
@@ -1586,7 +1624,7 @@
         <v>1967446</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="32" t="s">
         <v>25</v>
       </c>
@@ -1621,7 +1659,7 @@
         <v>3073011</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="32" t="s">
         <v>15</v>
       </c>
@@ -1656,7 +1694,7 @@
         <v>565247</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="32" t="s">
         <v>37</v>
       </c>
@@ -1691,7 +1729,7 @@
         <v>2116572</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="32" t="s">
         <v>49</v>
       </c>
@@ -1726,7 +1764,7 @@
         <v>7114999</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="32" t="s">
         <v>31</v>
       </c>
@@ -1761,7 +1799,7 @@
         <v>1659087</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="32" t="s">
         <v>47</v>
       </c>
@@ -1796,7 +1834,7 @@
         <v>1084234</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="32" t="s">
         <v>41</v>
       </c>
@@ -1831,7 +1869,7 @@
         <v>1622599</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="32" t="s">
         <v>23</v>
       </c>
@@ -1866,7 +1904,7 @@
         <v>396876</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="32" t="s">
         <v>21</v>
       </c>
@@ -1901,7 +1939,7 @@
         <v>520065</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="32" t="s">
         <v>17</v>
       </c>
@@ -1936,7 +1974,7 @@
         <v>1050795</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="32" t="s">
         <v>13</v>
       </c>
@@ -1980,24 +2018,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.69921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.296875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.19921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>55</v>
       </c>
@@ -2032,7 +2070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
@@ -2072,7 +2110,7 @@
         <v>116875.9</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>3</v>
       </c>
@@ -2112,7 +2150,7 @@
         <v>342469.60000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>5</v>
       </c>
@@ -2152,7 +2190,7 @@
         <v>131326.9</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>7</v>
       </c>
@@ -2192,7 +2230,7 @@
         <v>561290.9</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>9</v>
       </c>
@@ -2232,7 +2270,7 @@
         <v>1990077.8</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>11</v>
       </c>
@@ -2272,7 +2310,7 @@
         <v>1241752.5999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>13</v>
       </c>
@@ -2312,7 +2350,7 @@
         <v>457984.5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>15</v>
       </c>
@@ -2352,7 +2390,7 @@
         <v>564158.80000000005</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>17</v>
       </c>
@@ -2392,7 +2430,7 @@
         <v>1044033</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>19</v>
       </c>
@@ -2432,7 +2470,7 @@
         <v>814318.1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>21</v>
       </c>
@@ -2472,7 +2510,7 @@
         <v>499973.30000000005</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>23</v>
       </c>
@@ -2512,7 +2550,7 @@
         <v>402154</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
         <v>25</v>
       </c>
@@ -2552,7 +2590,7 @@
         <v>3305207.5</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>27</v>
       </c>
@@ -2592,7 +2630,7 @@
         <v>1140272.2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
         <v>29</v>
       </c>
@@ -2632,7 +2670,7 @@
         <v>483044.70000000007</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
         <v>31</v>
       </c>
@@ -2672,7 +2710,7 @@
         <v>1745776.4</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
         <v>33</v>
       </c>
@@ -2712,7 +2750,7 @@
         <v>1247588</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
         <v>35</v>
       </c>
@@ -2752,7 +2790,7 @@
         <v>393779.4</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
         <v>37</v>
       </c>
@@ -2792,7 +2830,7 @@
         <v>2180486.2999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
         <v>39</v>
       </c>
@@ -2832,7 +2870,7 @@
         <v>445655.7</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
         <v>41</v>
       </c>
@@ -2872,7 +2910,7 @@
         <v>1539896.5999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
         <v>43</v>
       </c>
@@ -2912,7 +2950,7 @@
         <v>277969.10000000003</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
         <v>45</v>
       </c>
@@ -2952,7 +2990,7 @@
         <v>73848.700000000012</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
         <v>47</v>
       </c>
@@ -2992,7 +3030,7 @@
         <v>1135364.2</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
         <v>49</v>
       </c>
@@ -3032,7 +3070,7 @@
         <v>7054850.7999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
         <v>51</v>
       </c>
@@ -3072,7 +3110,7 @@
         <v>324566.09999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="14" t="s">
         <v>53</v>
       </c>
@@ -3131,22 +3169,22 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.69921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.296875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.19921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.69921875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>55</v>
       </c>
@@ -3181,7 +3219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>1</v>
       </c>
@@ -3221,7 +3259,7 @@
         <v>116077.5</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>3</v>
       </c>
@@ -3261,7 +3299,7 @@
         <v>351779.5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>5</v>
       </c>
@@ -3301,7 +3339,7 @@
         <v>126402.4</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>7</v>
       </c>
@@ -3341,7 +3379,7 @@
         <v>577331</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>9</v>
       </c>
@@ -3381,7 +3419,7 @@
         <v>2061788.6</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>11</v>
       </c>
@@ -3421,7 +3459,7 @@
         <v>1234420.8</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>13</v>
       </c>
@@ -3461,7 +3499,7 @@
         <v>447357.2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>15</v>
       </c>
@@ -3501,7 +3539,7 @@
         <v>567121.30000000005</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>17</v>
       </c>
@@ -3541,7 +3579,7 @@
         <v>1062756.8999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>19</v>
       </c>
@@ -3581,7 +3619,7 @@
         <v>875343.2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>21</v>
       </c>
@@ -3621,7 +3659,7 @@
         <v>494873.10000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>23</v>
       </c>
@@ -3661,7 +3699,7 @@
         <v>391603.10000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
         <v>25</v>
       </c>
@@ -3701,7 +3739,7 @@
         <v>3255844.9000000004</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>27</v>
       </c>
@@ -3741,7 +3779,7 @@
         <v>1173080.7</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
         <v>29</v>
       </c>
@@ -3781,7 +3819,7 @@
         <v>477923.39999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
         <v>31</v>
       </c>
@@ -3821,7 +3859,7 @@
         <v>1724084.4000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
         <v>33</v>
       </c>
@@ -3861,7 +3899,7 @@
         <v>1196650.3999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
         <v>35</v>
       </c>
@@ -3901,7 +3939,7 @@
         <v>387319.19999999995</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
         <v>37</v>
       </c>
@@ -3941,7 +3979,7 @@
         <v>2105287.4</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
         <v>39</v>
       </c>
@@ -3981,7 +4019,7 @@
         <v>440955.80000000005</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="20" t="s">
         <v>41</v>
       </c>
@@ -4021,7 +4059,7 @@
         <v>1640078.2</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
         <v>43</v>
       </c>
@@ -4061,7 +4099,7 @@
         <v>262651.09999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="20" t="s">
         <v>45</v>
       </c>
@@ -4101,7 +4139,7 @@
         <v>69074.5</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
         <v>47</v>
       </c>
@@ -4141,7 +4179,7 @@
         <v>1144834.3</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="20" t="s">
         <v>49</v>
       </c>
@@ -4181,7 +4219,7 @@
         <v>6910690.2999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="20" t="s">
         <v>51</v>
       </c>
@@ -4221,7 +4259,7 @@
         <v>300033.90000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="20" t="s">
         <v>53</v>
       </c>
@@ -4276,26 +4314,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.69921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.296875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.19921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.69921875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>55</v>
       </c>
@@ -4330,7 +4368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>1</v>
       </c>
@@ -4341,36 +4379,31 @@
         <v>24967.599999999999</v>
       </c>
       <c r="D2" s="3">
-        <f>C2/K2</f>
         <v>0.24113639568327255</v>
       </c>
       <c r="E2" s="4">
         <v>5726.7</v>
       </c>
       <c r="F2" s="3">
-        <f>E2/K2</f>
         <v>5.5308311458025478E-2</v>
       </c>
       <c r="G2" s="4">
         <v>57182.8</v>
       </c>
       <c r="H2" s="3">
-        <f>G2/K2</f>
         <v>0.55226991329072239</v>
       </c>
       <c r="I2" s="4">
         <v>15664.3</v>
       </c>
       <c r="J2" s="3">
-        <f>I2/K2</f>
         <v>0.15128537956797955</v>
       </c>
       <c r="K2" s="21">
-        <f>SUM(C2,E2,G2,I2)</f>
         <v>103541.40000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>3</v>
       </c>
@@ -4381,36 +4414,31 @@
         <v>66746.5</v>
       </c>
       <c r="D3" s="3">
-        <f t="shared" ref="D3:D20" si="0">C3/K3</f>
         <v>0.16722880204282886</v>
       </c>
       <c r="E3" s="4">
         <v>26463.9</v>
       </c>
       <c r="F3" s="3">
-        <f t="shared" ref="F3:F28" si="1">E3/K3</f>
         <v>6.6303495979283089E-2</v>
       </c>
       <c r="G3" s="4">
         <v>231279.1</v>
       </c>
       <c r="H3" s="3">
-        <f t="shared" ref="H3:H28" si="2">G3/K3</f>
         <v>0.57945400628562727</v>
       </c>
       <c r="I3" s="4">
         <v>74643.3</v>
       </c>
       <c r="J3" s="3">
-        <f t="shared" ref="J3:J28" si="3">I3/K3</f>
         <v>0.18701369569226084</v>
       </c>
       <c r="K3" s="21">
-        <f t="shared" ref="K3:K28" si="4">SUM(C3,E3,G3,I3)</f>
         <v>399132.8</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>5</v>
       </c>
@@ -4421,36 +4449,31 @@
         <v>14474.7</v>
       </c>
       <c r="D4" s="3">
-        <f t="shared" si="0"/>
         <v>0.13845213522008368</v>
       </c>
       <c r="E4" s="4">
         <v>13036.6</v>
       </c>
       <c r="F4" s="3">
-        <f t="shared" si="1"/>
         <v>0.12469654680305242</v>
       </c>
       <c r="G4" s="4">
         <v>58587.9</v>
       </c>
       <c r="H4" s="3">
-        <f t="shared" si="2"/>
         <v>0.56039985996675168</v>
       </c>
       <c r="I4" s="4">
         <v>18447.400000000001</v>
       </c>
       <c r="J4" s="3">
-        <f t="shared" si="3"/>
         <v>0.17645145801011225</v>
       </c>
       <c r="K4" s="21">
-        <f t="shared" si="4"/>
         <v>104546.6</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>7</v>
       </c>
@@ -4458,39 +4481,34 @@
         <v>8</v>
       </c>
       <c r="C5" s="2">
-        <v>391881.1</v>
+        <v>115455</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" si="0"/>
-        <v>0.1809464245312204</v>
+        <v>0.19965528314804271</v>
       </c>
       <c r="E5" s="4">
-        <v>225990.8</v>
+        <v>53710</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" si="1"/>
-        <v>0.10434855683764827</v>
+        <v>9.2880215303636687E-2</v>
       </c>
       <c r="G5" s="4">
-        <v>1196219.8999999999</v>
+        <v>319067</v>
       </c>
       <c r="H5" s="3">
-        <f t="shared" si="2"/>
-        <v>0.55234027325659241</v>
+        <v>0.55175966591482861</v>
       </c>
       <c r="I5" s="4">
-        <v>351638.2</v>
+        <v>90039.7</v>
       </c>
       <c r="J5" s="3">
-        <f t="shared" si="3"/>
-        <v>0.16236474537453885</v>
+        <v>0.15570483563349202</v>
       </c>
       <c r="K5" s="21">
-        <f t="shared" si="4"/>
-        <v>2165730</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>578271.69999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>9</v>
       </c>
@@ -4498,39 +4516,34 @@
         <v>10</v>
       </c>
       <c r="C6" s="2">
-        <v>160088.70000000001</v>
+        <v>391881</v>
       </c>
       <c r="D6" s="3">
-        <f t="shared" si="0"/>
-        <v>0.13594216352321745</v>
+        <v>0.18094637835741298</v>
       </c>
       <c r="E6" s="4">
-        <v>67007</v>
+        <v>225991</v>
       </c>
       <c r="F6" s="3">
-        <f t="shared" si="1"/>
-        <v>5.6900184405271767E-2</v>
+        <v>0.10434864918526317</v>
       </c>
       <c r="G6" s="4">
-        <v>749490.4</v>
+        <v>1196220</v>
       </c>
       <c r="H6" s="3">
-        <f t="shared" si="2"/>
-        <v>0.63644308758757884</v>
+        <v>0.55234031943039996</v>
       </c>
       <c r="I6" s="4">
-        <v>201037.5</v>
+        <v>351638</v>
       </c>
       <c r="J6" s="3">
-        <f t="shared" si="3"/>
-        <v>0.17071456448393185</v>
+        <v>0.16236465302692396</v>
       </c>
       <c r="K6" s="21">
-        <f t="shared" si="4"/>
-        <v>1177623.6000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2165730</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>11</v>
       </c>
@@ -4538,39 +4551,34 @@
         <v>12</v>
       </c>
       <c r="C7" s="2">
-        <v>78188</v>
+        <v>160089</v>
       </c>
       <c r="D7" s="3">
-        <f t="shared" si="0"/>
-        <v>0.19499557576416579</v>
+        <v>0.13594248753633378</v>
       </c>
       <c r="E7" s="4">
-        <v>35876.300000000003</v>
+        <v>67007</v>
       </c>
       <c r="F7" s="3">
-        <f t="shared" si="1"/>
-        <v>8.9473062040056547E-2</v>
+        <v>5.6900213395967979E-2</v>
       </c>
       <c r="G7" s="4">
-        <v>225223.2</v>
+        <v>749490</v>
       </c>
       <c r="H7" s="3">
-        <f t="shared" si="2"/>
-        <v>0.56169140481209223</v>
+        <v>0.6364430721886376</v>
       </c>
       <c r="I7" s="4">
-        <v>61685.7</v>
+        <v>201037</v>
       </c>
       <c r="J7" s="3">
-        <f t="shared" si="3"/>
-        <v>0.15383995738368547</v>
+        <v>0.17071422687906063</v>
       </c>
       <c r="K7" s="21">
-        <f t="shared" si="4"/>
-        <v>400973.2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1177623</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>13</v>
       </c>
@@ -4578,39 +4586,34 @@
         <v>14</v>
       </c>
       <c r="C8" s="2">
-        <v>89265.8</v>
+        <v>78188</v>
       </c>
       <c r="D8" s="3">
-        <f t="shared" si="0"/>
-        <v>0.16349760300906888</v>
+        <v>0.1949956730253658</v>
       </c>
       <c r="E8" s="4">
-        <v>34710.400000000001</v>
+        <v>35876.300000000003</v>
       </c>
       <c r="F8" s="3">
-        <f t="shared" si="1"/>
-        <v>6.3574932387162664E-2</v>
+        <v>8.9473106668030031E-2</v>
       </c>
       <c r="G8" s="4">
-        <v>332085.40000000002</v>
+        <v>225223</v>
       </c>
       <c r="H8" s="3">
-        <f t="shared" si="2"/>
-        <v>0.60824153140741299</v>
+        <v>0.56169118618959379</v>
       </c>
       <c r="I8" s="4">
-        <v>89914.6</v>
+        <v>61685.7</v>
       </c>
       <c r="J8" s="3">
-        <f t="shared" si="3"/>
-        <v>0.16468593319635544</v>
+        <v>0.15384003411701036</v>
       </c>
       <c r="K8" s="21">
-        <f t="shared" si="4"/>
-        <v>545976.20000000007</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>400973</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>15</v>
       </c>
@@ -4621,36 +4624,31 @@
         <v>89265.8</v>
       </c>
       <c r="D9" s="3">
-        <f t="shared" si="0"/>
         <v>0.16349760300906888</v>
       </c>
       <c r="E9" s="4">
         <v>34710.400000000001</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" si="1"/>
         <v>6.3574932387162664E-2</v>
       </c>
       <c r="G9" s="4">
         <v>332085.40000000002</v>
       </c>
       <c r="H9" s="3">
-        <f t="shared" si="2"/>
         <v>0.60824153140741299</v>
       </c>
       <c r="I9" s="4">
         <v>89914.6</v>
       </c>
       <c r="J9" s="3">
-        <f t="shared" si="3"/>
         <v>0.16468593319635544</v>
       </c>
       <c r="K9" s="21">
-        <f t="shared" si="4"/>
         <v>545976.20000000007</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>17</v>
       </c>
@@ -4661,36 +4659,31 @@
         <v>217325.7</v>
       </c>
       <c r="D10" s="3">
-        <f t="shared" si="0"/>
         <v>0.21167406594157961</v>
       </c>
       <c r="E10" s="4">
         <v>68505.600000000006</v>
       </c>
       <c r="F10" s="3">
-        <f t="shared" si="1"/>
         <v>6.6724086897074195E-2</v>
       </c>
       <c r="G10" s="4">
         <v>604082.4</v>
       </c>
       <c r="H10" s="3">
-        <f t="shared" si="2"/>
         <v>0.58837301695909716</v>
       </c>
       <c r="I10" s="4">
         <v>136786</v>
       </c>
       <c r="J10" s="3">
-        <f t="shared" si="3"/>
         <v>0.13322883020224902</v>
       </c>
       <c r="K10" s="21">
-        <f t="shared" si="4"/>
         <v>1026699.7000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>19</v>
       </c>
@@ -4701,36 +4694,31 @@
         <v>149969.29999999999</v>
       </c>
       <c r="D11" s="3">
-        <f t="shared" si="0"/>
         <v>0.16385395657199797</v>
       </c>
       <c r="E11" s="4">
         <v>45140.5</v>
       </c>
       <c r="F11" s="3">
-        <f t="shared" si="1"/>
         <v>4.9319757621314998E-2</v>
       </c>
       <c r="G11" s="4">
         <v>568020.6</v>
       </c>
       <c r="H11" s="3">
-        <f t="shared" si="2"/>
         <v>0.62060983630916622</v>
       </c>
       <c r="I11" s="4">
         <v>152131.6</v>
       </c>
       <c r="J11" s="3">
-        <f t="shared" si="3"/>
         <v>0.16621644949752096</v>
       </c>
       <c r="K11" s="21">
-        <f t="shared" si="4"/>
         <v>915261.99999999988</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>21</v>
       </c>
@@ -4741,36 +4729,31 @@
         <v>109358.8</v>
       </c>
       <c r="D12" s="3">
-        <f t="shared" si="0"/>
         <v>0.21389951345932862</v>
       </c>
       <c r="E12" s="4">
         <v>29625.200000000001</v>
       </c>
       <c r="F12" s="3">
-        <f t="shared" si="1"/>
         <v>5.7945184714310163E-2</v>
       </c>
       <c r="G12" s="4">
         <v>313415.5</v>
       </c>
       <c r="H12" s="3">
-        <f t="shared" si="2"/>
         <v>0.61302266448253095</v>
       </c>
       <c r="I12" s="4">
         <v>58863</v>
       </c>
       <c r="J12" s="3">
-        <f t="shared" si="3"/>
         <v>0.11513263734383022</v>
       </c>
       <c r="K12" s="21">
-        <f t="shared" si="4"/>
         <v>511262.5</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>23</v>
       </c>
@@ -4781,36 +4764,31 @@
         <v>87186.7</v>
       </c>
       <c r="D13" s="3">
-        <f t="shared" si="0"/>
         <v>0.2185749895521763</v>
       </c>
       <c r="E13" s="4">
         <v>25085.4</v>
       </c>
       <c r="F13" s="3">
-        <f t="shared" si="1"/>
         <v>6.2888502981672242E-2</v>
       </c>
       <c r="G13" s="4">
         <v>250363.9</v>
       </c>
       <c r="H13" s="3">
-        <f t="shared" si="2"/>
         <v>0.62765636073784314</v>
       </c>
       <c r="I13" s="4">
         <v>36250.9</v>
       </c>
       <c r="J13" s="3">
-        <f t="shared" si="3"/>
         <v>9.08801467283082E-2</v>
       </c>
       <c r="K13" s="21">
-        <f t="shared" si="4"/>
         <v>398886.9</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
         <v>25</v>
       </c>
@@ -4821,36 +4799,31 @@
         <v>614122</v>
       </c>
       <c r="D14" s="3">
-        <f t="shared" si="0"/>
         <v>0.19115232679234603</v>
       </c>
       <c r="E14" s="4">
         <v>222882.5</v>
       </c>
       <c r="F14" s="3">
-        <f t="shared" si="1"/>
         <v>6.9374665744420597E-2</v>
       </c>
       <c r="G14" s="4">
         <v>1960533.6</v>
       </c>
       <c r="H14" s="3">
-        <f t="shared" si="2"/>
         <v>0.61023796476038084</v>
       </c>
       <c r="I14" s="4">
         <v>415198.1</v>
       </c>
       <c r="J14" s="3">
-        <f t="shared" si="3"/>
         <v>0.12923504270285247</v>
       </c>
       <c r="K14" s="21">
-        <f t="shared" si="4"/>
         <v>3212736.2</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>27</v>
       </c>
@@ -4861,36 +4834,31 @@
         <v>220339.1</v>
       </c>
       <c r="D15" s="3">
-        <f t="shared" si="0"/>
         <v>0.18081957212041971</v>
       </c>
       <c r="E15" s="4">
         <v>76548.100000000006</v>
       </c>
       <c r="F15" s="3">
-        <f t="shared" si="1"/>
         <v>6.2818604090835908E-2</v>
       </c>
       <c r="G15" s="4">
         <v>751284.1</v>
       </c>
       <c r="H15" s="3">
-        <f t="shared" si="2"/>
         <v>0.61653546512114565</v>
       </c>
       <c r="I15" s="4">
         <v>170386.5</v>
       </c>
       <c r="J15" s="3">
-        <f t="shared" si="3"/>
         <v>0.13982635866759868</v>
       </c>
       <c r="K15" s="21">
-        <f t="shared" si="4"/>
         <v>1218557.8</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
         <v>29</v>
       </c>
@@ -4901,36 +4869,31 @@
         <v>92420.800000000003</v>
       </c>
       <c r="D16" s="3">
-        <f t="shared" si="0"/>
         <v>0.18629244556606855</v>
       </c>
       <c r="E16" s="4">
         <v>31675.599999999999</v>
       </c>
       <c r="F16" s="3">
-        <f t="shared" si="1"/>
         <v>6.3848451742168008E-2</v>
       </c>
       <c r="G16" s="4">
         <v>299352</v>
       </c>
       <c r="H16" s="3">
-        <f t="shared" si="2"/>
         <v>0.60340330493886385</v>
       </c>
       <c r="I16" s="4">
         <v>72657.600000000006</v>
       </c>
       <c r="J16" s="3">
-        <f t="shared" si="3"/>
         <v>0.1464557977528996</v>
       </c>
       <c r="K16" s="21">
-        <f t="shared" si="4"/>
         <v>496106</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
         <v>31</v>
       </c>
@@ -4941,36 +4904,31 @@
         <v>356412.1</v>
       </c>
       <c r="D17" s="3">
-        <f t="shared" si="0"/>
         <v>0.20997339779211396</v>
       </c>
       <c r="E17" s="4">
         <v>100924.6</v>
       </c>
       <c r="F17" s="3">
-        <f t="shared" si="1"/>
         <v>5.9457805116072064E-2</v>
       </c>
       <c r="G17" s="4">
         <v>1061051.8999999999</v>
       </c>
       <c r="H17" s="3">
-        <f t="shared" si="2"/>
         <v>0.62509851005837991</v>
       </c>
       <c r="I17" s="4">
         <v>179026.9</v>
       </c>
       <c r="J17" s="3">
-        <f t="shared" si="3"/>
         <v>0.10547028703343407</v>
       </c>
       <c r="K17" s="21">
-        <f t="shared" si="4"/>
         <v>1697415.4999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
         <v>33</v>
       </c>
@@ -4981,36 +4939,31 @@
         <v>163398.29999999999</v>
       </c>
       <c r="D18" s="3">
-        <f t="shared" si="0"/>
         <v>0.13300048137884352</v>
       </c>
       <c r="E18" s="4">
         <v>74606.100000000006</v>
       </c>
       <c r="F18" s="3">
-        <f t="shared" si="1"/>
         <v>6.0726746935544244E-2</v>
       </c>
       <c r="G18" s="4">
         <v>751467.2</v>
       </c>
       <c r="H18" s="3">
-        <f t="shared" si="2"/>
         <v>0.6116679264130146</v>
       </c>
       <c r="I18" s="4">
         <v>239082.6</v>
       </c>
       <c r="J18" s="3">
-        <f t="shared" si="3"/>
         <v>0.19460484527259767</v>
       </c>
       <c r="K18" s="21">
-        <f t="shared" si="4"/>
         <v>1228554.2</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
         <v>35</v>
       </c>
@@ -5021,36 +4974,31 @@
         <v>83480.600000000006</v>
       </c>
       <c r="D19" s="3">
-        <f t="shared" si="0"/>
         <v>0.19949152489719019</v>
       </c>
       <c r="E19" s="4">
         <v>20658.400000000001</v>
       </c>
       <c r="F19" s="3">
-        <f t="shared" si="1"/>
         <v>4.9366867487010323E-2</v>
       </c>
       <c r="G19" s="4">
         <v>255111.4</v>
       </c>
       <c r="H19" s="3">
-        <f t="shared" si="2"/>
         <v>0.60963340230732699</v>
       </c>
       <c r="I19" s="4">
         <v>59216.5</v>
       </c>
       <c r="J19" s="3">
-        <f t="shared" si="3"/>
         <v>0.14150820530847241</v>
       </c>
       <c r="K19" s="21">
-        <f t="shared" si="4"/>
         <v>418466.9</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
         <v>37</v>
       </c>
@@ -5061,36 +5009,31 @@
         <v>291567.40000000002</v>
       </c>
       <c r="D20" s="3">
-        <f t="shared" si="0"/>
         <v>0.1406628139915134</v>
       </c>
       <c r="E20" s="4">
         <v>117542.8</v>
       </c>
       <c r="F20" s="3">
-        <f t="shared" si="1"/>
         <v>5.6706960423015942E-2</v>
       </c>
       <c r="G20" s="4">
         <v>1316404.5</v>
       </c>
       <c r="H20" s="3">
-        <f t="shared" si="2"/>
         <v>0.6350818415264915</v>
       </c>
       <c r="I20" s="4">
         <v>347296.1</v>
       </c>
       <c r="J20" s="3">
-        <f t="shared" si="3"/>
         <v>0.16754838405897923</v>
       </c>
       <c r="K20" s="21">
-        <f t="shared" si="4"/>
         <v>2072810.7999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
         <v>39</v>
       </c>
@@ -5101,36 +5044,31 @@
         <v>74043.199999999997</v>
       </c>
       <c r="D21" s="3">
-        <f>C21/K21</f>
         <v>0.16690286172839783</v>
       </c>
       <c r="E21" s="4">
         <v>30918.9</v>
       </c>
       <c r="F21" s="3">
-        <f t="shared" si="1"/>
         <v>6.9695162979100861E-2</v>
       </c>
       <c r="G21" s="4">
         <v>254817.5</v>
       </c>
       <c r="H21" s="3">
-        <f t="shared" si="2"/>
         <v>0.57439130086862833</v>
       </c>
       <c r="I21" s="4">
         <v>83850.899999999994</v>
       </c>
       <c r="J21" s="3">
-        <f t="shared" si="3"/>
         <v>0.18901067442387301</v>
       </c>
       <c r="K21" s="21">
-        <f t="shared" si="4"/>
         <v>443630.5</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="20" t="s">
         <v>41</v>
       </c>
@@ -5141,36 +5079,31 @@
         <v>390608.6</v>
       </c>
       <c r="D22" s="3">
-        <f t="shared" ref="D22:D28" si="5">C22/K22</f>
         <v>0.22945799877319625</v>
       </c>
       <c r="E22" s="4">
         <v>110917.9</v>
       </c>
       <c r="F22" s="3">
-        <f t="shared" si="1"/>
         <v>6.5157293930869692E-2</v>
       </c>
       <c r="G22" s="4">
         <v>1029362.6</v>
       </c>
       <c r="H22" s="3">
-        <f t="shared" si="2"/>
         <v>0.60468582158194706</v>
       </c>
       <c r="I22" s="4">
         <v>171420.7</v>
       </c>
       <c r="J22" s="3">
-        <f t="shared" si="3"/>
         <v>0.10069888571398697</v>
       </c>
       <c r="K22" s="21">
-        <f t="shared" si="4"/>
         <v>1702309.8</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
         <v>43</v>
       </c>
@@ -5181,36 +5114,31 @@
         <v>61992.800000000003</v>
       </c>
       <c r="D23" s="3">
-        <f t="shared" si="5"/>
         <v>0.22698531783649081</v>
       </c>
       <c r="E23" s="4">
         <v>15154.3</v>
       </c>
       <c r="F23" s="3">
-        <f t="shared" si="1"/>
         <v>5.5487146928184121E-2</v>
       </c>
       <c r="G23" s="4">
         <v>170625.9</v>
       </c>
       <c r="H23" s="3">
-        <f t="shared" si="2"/>
         <v>0.62474310149948531</v>
       </c>
       <c r="I23" s="4">
         <v>25340.7</v>
       </c>
       <c r="J23" s="3">
-        <f t="shared" si="3"/>
         <v>9.2784433735839694E-2</v>
       </c>
       <c r="K23" s="21">
-        <f t="shared" si="4"/>
         <v>273113.7</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="20" t="s">
         <v>45</v>
       </c>
@@ -5221,36 +5149,31 @@
         <v>14216</v>
       </c>
       <c r="D24" s="3">
-        <f t="shared" si="5"/>
         <v>0.2037940441563319</v>
       </c>
       <c r="E24" s="4">
         <v>5101.3</v>
       </c>
       <c r="F24" s="3">
-        <f t="shared" si="1"/>
         <v>7.3129892899176707E-2</v>
       </c>
       <c r="G24" s="4">
         <v>41805.300000000003</v>
       </c>
       <c r="H24" s="3">
-        <f t="shared" si="2"/>
         <v>0.59930157246544058</v>
       </c>
       <c r="I24" s="4">
         <v>8634.1</v>
       </c>
       <c r="J24" s="3">
-        <f t="shared" si="3"/>
         <v>0.12377449047905074</v>
       </c>
       <c r="K24" s="21">
-        <f t="shared" si="4"/>
         <v>69756.700000000012</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
         <v>47</v>
       </c>
@@ -5261,36 +5184,31 @@
         <v>241180</v>
       </c>
       <c r="D25" s="3">
-        <f t="shared" si="5"/>
         <v>0.2237800909205204</v>
       </c>
       <c r="E25" s="4">
         <v>50590.5</v>
       </c>
       <c r="F25" s="3">
-        <f t="shared" si="1"/>
         <v>4.6940652996577605E-2</v>
       </c>
       <c r="G25" s="4">
         <v>709946.8</v>
       </c>
       <c r="H25" s="3">
-        <f t="shared" si="2"/>
         <v>0.65872775293445773</v>
       </c>
       <c r="I25" s="4">
         <v>76037.2</v>
       </c>
       <c r="J25" s="3">
-        <f t="shared" si="3"/>
         <v>7.0551503148444286E-2</v>
       </c>
       <c r="K25" s="21">
-        <f t="shared" si="4"/>
         <v>1077754.5</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="20" t="s">
         <v>49</v>
       </c>
@@ -5301,36 +5219,31 @@
         <v>1121492.2</v>
       </c>
       <c r="D26" s="3">
-        <f t="shared" si="5"/>
         <v>0.16052702699201649</v>
       </c>
       <c r="E26" s="4">
         <v>611464.30000000005</v>
       </c>
       <c r="F26" s="3">
-        <f t="shared" si="1"/>
         <v>8.752316439717947E-2</v>
       </c>
       <c r="G26" s="4">
         <v>4202489.9000000004</v>
       </c>
       <c r="H26" s="3">
-        <f t="shared" si="2"/>
         <v>0.60153178917425976</v>
       </c>
       <c r="I26" s="4">
         <v>1050867.5</v>
       </c>
       <c r="J26" s="3">
-        <f t="shared" si="3"/>
         <v>0.15041801943654434</v>
       </c>
       <c r="K26" s="21">
-        <f t="shared" si="4"/>
         <v>6986313.9000000004</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="20" t="s">
         <v>51</v>
       </c>
@@ -5341,36 +5254,31 @@
         <v>54995.6</v>
       </c>
       <c r="D27" s="3">
-        <f t="shared" si="5"/>
         <v>0.17909605918067742</v>
       </c>
       <c r="E27" s="4">
         <v>15008.5</v>
       </c>
       <c r="F27" s="3">
-        <f t="shared" si="1"/>
         <v>4.8875968335888642E-2</v>
       </c>
       <c r="G27" s="4">
         <v>179943.1</v>
       </c>
       <c r="H27" s="3">
-        <f t="shared" si="2"/>
         <v>0.58599415383693532</v>
       </c>
       <c r="I27" s="4">
         <v>57126</v>
       </c>
       <c r="J27" s="3">
-        <f t="shared" si="3"/>
         <v>0.18603381864649862</v>
       </c>
       <c r="K27" s="21">
-        <f t="shared" si="4"/>
         <v>307073.2</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="20" t="s">
         <v>53</v>
       </c>
@@ -5381,32 +5289,27 @@
         <v>41758.5</v>
       </c>
       <c r="D28" s="3">
-        <f t="shared" si="5"/>
         <v>0.19103092241148606</v>
       </c>
       <c r="E28" s="4">
         <v>14120.2</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" si="1"/>
         <v>6.4595108316502406E-2</v>
       </c>
       <c r="G28" s="4">
         <v>133163</v>
       </c>
       <c r="H28" s="3">
-        <f t="shared" si="2"/>
         <v>0.60917539473593918</v>
       </c>
       <c r="I28" s="4">
         <v>29553.8</v>
       </c>
       <c r="J28" s="3">
-        <f t="shared" si="3"/>
         <v>0.13519857453607234</v>
       </c>
       <c r="K28" s="21">
-        <f t="shared" si="4"/>
         <v>218595.5</v>
       </c>
     </row>
@@ -5429,26 +5332,26 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.875" customWidth="1"/>
-    <col min="2" max="2" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.796875" customWidth="1"/>
+    <col min="2" max="2" width="20.69921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="31.625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="34.375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.19921875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.19921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.69921875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.19921875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.69921875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.69921875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>55</v>
       </c>
@@ -5495,7 +5398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>1</v>
       </c>
@@ -5549,7 +5452,7 @@
         <v>226004</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>3</v>
       </c>
@@ -5603,7 +5506,7 @@
         <v>817999</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>5</v>
       </c>
@@ -5657,7 +5560,7 @@
         <v>209954</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
         <v>7</v>
       </c>
@@ -5711,7 +5614,7 @@
         <v>1074692</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="22" t="s">
         <v>9</v>
       </c>
@@ -5765,7 +5668,7 @@
         <v>3625890</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
         <v>11</v>
       </c>
@@ -5819,7 +5722,7 @@
         <v>2292212</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
         <v>13</v>
       </c>
@@ -5873,7 +5776,7 @@
         <v>727574</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
         <v>15</v>
       </c>
@@ -5927,7 +5830,7 @@
         <v>865331</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
         <v>17</v>
       </c>
@@ -5981,7 +5884,7 @@
         <v>1571118</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>19</v>
       </c>
@@ -6035,7 +5938,7 @@
         <v>1792607</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="22" t="s">
         <v>21</v>
       </c>
@@ -6089,7 +5992,7 @@
         <v>784689</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
         <v>23</v>
       </c>
@@ -6143,7 +6046,7 @@
         <v>634478</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
         <v>25</v>
       </c>
@@ -6197,7 +6100,7 @@
         <v>4871826</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="22" t="s">
         <v>27</v>
       </c>
@@ -6251,7 +6154,7 @@
         <v>2139650</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
         <v>29</v>
       </c>
@@ -6305,7 +6208,7 @@
         <v>964483</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="22" t="s">
         <v>31</v>
       </c>
@@ -6359,7 +6262,7 @@
         <v>2614040</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="22" t="s">
         <v>33</v>
       </c>
@@ -6413,7 +6316,7 @@
         <v>2263021</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="22" t="s">
         <v>35</v>
       </c>
@@ -6467,7 +6370,7 @@
         <v>791948</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="22" t="s">
         <v>37</v>
       </c>
@@ -6521,7 +6424,7 @@
         <v>3591796</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="22" t="s">
         <v>39</v>
       </c>
@@ -6575,7 +6478,7 @@
         <v>884510</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
         <v>41</v>
       </c>
@@ -6629,7 +6532,7 @@
         <v>2390782</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="22" t="s">
         <v>43</v>
       </c>
@@ -6683,7 +6586,7 @@
         <v>454442</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="22" t="s">
         <v>45</v>
       </c>
@@ -6737,7 +6640,7 @@
         <v>134330</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="22" t="s">
         <v>47</v>
       </c>
@@ -6791,7 +6694,7 @@
         <v>1521962</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="22" t="s">
         <v>49</v>
       </c>
@@ -6845,7 +6748,7 @@
         <v>10147915</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="22" t="s">
         <v>51</v>
       </c>
@@ -6899,7 +6802,7 @@
         <v>589482</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="22" t="s">
         <v>53</v>
       </c>
@@ -6972,9 +6875,9 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>55</v>
       </c>
@@ -7021,7 +6924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>1</v>
       </c>
@@ -7075,7 +6978,7 @@
         <v>217716</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>3</v>
       </c>
@@ -7129,7 +7032,7 @@
         <v>905825</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>5</v>
       </c>
@@ -7183,7 +7086,7 @@
         <v>215775</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
         <v>7</v>
       </c>
@@ -7237,7 +7140,7 @@
         <v>1073723</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="22" t="s">
         <v>9</v>
       </c>
@@ -7291,7 +7194,7 @@
         <v>3719035</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
         <v>11</v>
       </c>
@@ -7345,7 +7248,7 @@
         <v>2300480</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
         <v>13</v>
       </c>
@@ -7399,7 +7302,7 @@
         <v>710230</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
         <v>15</v>
       </c>
@@ -7453,7 +7356,7 @@
         <v>905677</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
         <v>17</v>
       </c>
@@ -7507,7 +7410,7 @@
         <v>1606357</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>19</v>
       </c>
@@ -7561,7 +7464,7 @@
         <v>1798538</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="22" t="s">
         <v>21</v>
       </c>
@@ -7615,7 +7518,7 @@
         <v>786950</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
         <v>23</v>
       </c>
@@ -7669,7 +7572,7 @@
         <v>621160</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
         <v>25</v>
       </c>
@@ -7723,7 +7626,7 @@
         <v>4961486</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="22" t="s">
         <v>27</v>
       </c>
@@ -7777,7 +7680,7 @@
         <v>2146988</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
         <v>29</v>
       </c>
@@ -7831,7 +7734,7 @@
         <v>980917</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="22" t="s">
         <v>31</v>
       </c>
@@ -7885,7 +7788,7 @@
         <v>2600936</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="22" t="s">
         <v>33</v>
       </c>
@@ -7939,7 +7842,7 @@
         <v>2274846</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="22" t="s">
         <v>35</v>
       </c>
@@ -7993,7 +7896,7 @@
         <v>822314</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="22" t="s">
         <v>37</v>
       </c>
@@ -8047,7 +7950,7 @@
         <v>3649085</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="22" t="s">
         <v>39</v>
       </c>
@@ -8101,7 +8004,7 @@
         <v>913566</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
         <v>41</v>
       </c>
@@ -8155,7 +8058,7 @@
         <v>2460684</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="22" t="s">
         <v>43</v>
       </c>
@@ -8209,7 +8112,7 @@
         <v>452622</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="22" t="s">
         <v>45</v>
       </c>
@@ -8263,7 +8166,7 @@
         <v>141819</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="22" t="s">
         <v>47</v>
       </c>
@@ -8317,7 +8220,7 @@
         <v>1530835</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="22" t="s">
         <v>49</v>
       </c>
@@ -8371,7 +8274,7 @@
         <v>10218686</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="22" t="s">
         <v>51</v>
       </c>
@@ -8425,7 +8328,7 @@
         <v>573979</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="22" t="s">
         <v>53</v>
       </c>
@@ -8498,9 +8401,9 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>55</v>
       </c>
@@ -8547,7 +8450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>1</v>
       </c>
@@ -8601,7 +8504,7 @@
         <v>220209</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>3</v>
       </c>
@@ -8655,7 +8558,7 @@
         <v>848704</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>5</v>
       </c>
@@ -8709,7 +8612,7 @@
         <v>215128</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
         <v>7</v>
       </c>
@@ -8763,7 +8666,7 @@
         <v>1047839</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="22" t="s">
         <v>9</v>
       </c>
@@ -8817,7 +8720,7 @@
         <v>3677120</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
         <v>11</v>
       </c>
@@ -8871,7 +8774,7 @@
         <v>2345589</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
         <v>13</v>
       </c>
@@ -8925,7 +8828,7 @@
         <v>704611</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
         <v>15</v>
       </c>
@@ -8979,7 +8882,7 @@
         <v>947827</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
         <v>17</v>
       </c>
@@ -9033,7 +8936,7 @@
         <v>1613576</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>19</v>
       </c>
@@ -9087,7 +8990,7 @@
         <v>1798449</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="22" t="s">
         <v>21</v>
       </c>
@@ -9141,7 +9044,7 @@
         <v>837131</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
         <v>23</v>
       </c>
@@ -9195,7 +9098,7 @@
         <v>637841</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
         <v>25</v>
       </c>
@@ -9249,7 +9152,7 @@
         <v>4974921</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="22" t="s">
         <v>27</v>
       </c>
@@ -9303,7 +9206,7 @@
         <v>2143398</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
         <v>29</v>
       </c>
@@ -9357,7 +9260,7 @@
         <v>988756</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="22" t="s">
         <v>31</v>
       </c>
@@ -9411,7 +9314,7 @@
         <v>2657461</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="22" t="s">
         <v>33</v>
       </c>
@@ -9465,7 +9368,7 @@
         <v>2287455</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="22" t="s">
         <v>35</v>
       </c>
@@ -9519,7 +9422,7 @@
         <v>792682</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="22" t="s">
         <v>37</v>
       </c>
@@ -9573,7 +9476,7 @@
         <v>3683133</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="22" t="s">
         <v>39</v>
       </c>
@@ -9627,7 +9530,7 @@
         <v>859593</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
         <v>41</v>
       </c>
@@ -9681,7 +9584,7 @@
         <v>2440311</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="22" t="s">
         <v>43</v>
       </c>
@@ -9735,7 +9638,7 @@
         <v>456967</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="22" t="s">
         <v>45</v>
       </c>
@@ -9789,7 +9692,7 @@
         <v>132454</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="22" t="s">
         <v>47</v>
       </c>
@@ -9843,7 +9746,7 @@
         <v>1534676</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="22" t="s">
         <v>49</v>
       </c>
@@ -9897,7 +9800,7 @@
         <v>10204111</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="22" t="s">
         <v>51</v>
       </c>
@@ -9951,7 +9854,7 @@
         <v>576340</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="22" t="s">
         <v>53</v>
       </c>
@@ -10024,9 +9927,9 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>55</v>
       </c>
@@ -10073,7 +9976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>1</v>
       </c>
@@ -10127,7 +10030,7 @@
         <v>221424</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>3</v>
       </c>
@@ -10181,7 +10084,7 @@
         <v>885418</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>5</v>
       </c>
@@ -10235,7 +10138,7 @@
         <v>206775</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
         <v>7</v>
       </c>
@@ -10289,7 +10192,7 @@
         <v>1021836</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="22" t="s">
         <v>9</v>
       </c>
@@ -10343,7 +10246,7 @@
         <v>3800359</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
         <v>11</v>
       </c>
@@ -10397,7 +10300,7 @@
         <v>2342955</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
         <v>13</v>
       </c>
@@ -10451,7 +10354,7 @@
         <v>734908</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
         <v>15</v>
       </c>
@@ -10505,7 +10408,7 @@
         <v>913994</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
         <v>17</v>
       </c>
@@ -10559,7 +10462,7 @@
         <v>1614353</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>19</v>
       </c>
@@ -10613,7 +10516,7 @@
         <v>1779850</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="22" t="s">
         <v>21</v>
       </c>
@@ -10667,7 +10570,7 @@
         <v>807309</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
         <v>23</v>
       </c>
@@ -10721,7 +10624,7 @@
         <v>680485</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
         <v>25</v>
       </c>
@@ -10775,7 +10678,7 @@
         <v>4986330</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="22" t="s">
         <v>27</v>
       </c>
@@ -10829,7 +10732,7 @@
         <v>2166594</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
         <v>29</v>
       </c>
@@ -10883,7 +10786,7 @@
         <v>1004403</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="22" t="s">
         <v>31</v>
       </c>
@@ -10937,7 +10840,7 @@
         <v>2619048</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="22" t="s">
         <v>33</v>
       </c>
@@ -10991,7 +10894,7 @@
         <v>2266140</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="22" t="s">
         <v>35</v>
       </c>
@@ -11045,7 +10948,7 @@
         <v>864364</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="22" t="s">
         <v>37</v>
       </c>
@@ -11099,7 +11002,7 @@
         <v>3627031</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="22" t="s">
         <v>39</v>
       </c>
@@ -11153,7 +11056,7 @@
         <v>924504</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
         <v>41</v>
       </c>
@@ -11207,7 +11110,7 @@
         <v>2562673</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="22" t="s">
         <v>43</v>
       </c>
@@ -11261,7 +11164,7 @@
         <v>469550</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="22" t="s">
         <v>45</v>
       </c>
@@ -11315,7 +11218,7 @@
         <v>138433</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="22" t="s">
         <v>47</v>
       </c>
@@ -11369,7 +11272,7 @@
         <v>1597801</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="22" t="s">
         <v>49</v>
       </c>
@@ -11423,7 +11326,7 @@
         <v>10332092</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="22" t="s">
         <v>51</v>
       </c>
@@ -11477,7 +11380,7 @@
         <v>597683</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="22" t="s">
         <v>53</v>
       </c>
@@ -11550,9 +11453,9 @@
       <selection sqref="A1:O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>55</v>
       </c>
@@ -11599,7 +11502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>1</v>
       </c>
@@ -11653,7 +11556,7 @@
         <v>206191</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>3</v>
       </c>
@@ -11707,7 +11610,7 @@
         <v>881561</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>5</v>
       </c>
@@ -11761,7 +11664,7 @@
         <v>208362</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
         <v>7</v>
       </c>
@@ -11815,7 +11718,7 @@
         <v>1011210</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="22" t="s">
         <v>9</v>
       </c>
@@ -11869,7 +11772,7 @@
         <v>3804673</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
         <v>11</v>
       </c>
@@ -11923,7 +11826,7 @@
         <v>2299341</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
         <v>13</v>
       </c>
@@ -11977,7 +11880,7 @@
         <v>715738</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
         <v>15</v>
       </c>
@@ -12031,7 +11934,7 @@
         <v>974251</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
         <v>17</v>
       </c>
@@ -12085,7 +11988,7 @@
         <v>1600442</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>19</v>
       </c>
@@ -12139,7 +12042,7 @@
         <v>1821700</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="22" t="s">
         <v>21</v>
       </c>
@@ -12193,7 +12096,7 @@
         <v>838124</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
         <v>23</v>
       </c>
@@ -12247,7 +12150,7 @@
         <v>638247</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
         <v>25</v>
       </c>
@@ -12301,7 +12204,7 @@
         <v>5021391</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="22" t="s">
         <v>27</v>
       </c>
@@ -12355,7 +12258,7 @@
         <v>2209363</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
         <v>29</v>
       </c>
@@ -12409,7 +12312,7 @@
         <v>1014906</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="22" t="s">
         <v>31</v>
       </c>
@@ -12463,7 +12366,7 @@
         <v>2724734</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="22" t="s">
         <v>33</v>
       </c>
@@ -12517,7 +12420,7 @@
         <v>2365793</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="22" t="s">
         <v>35</v>
       </c>
@@ -12571,7 +12474,7 @@
         <v>803380</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="22" t="s">
         <v>37</v>
       </c>
@@ -12625,7 +12528,7 @@
         <v>3696648</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="22" t="s">
         <v>39</v>
       </c>
@@ -12679,7 +12582,7 @@
         <v>869191</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
         <v>41</v>
       </c>
@@ -12733,7 +12636,7 @@
         <v>2570228</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="22" t="s">
         <v>43</v>
       </c>
@@ -12787,7 +12690,7 @@
         <v>458040</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="22" t="s">
         <v>45</v>
       </c>
@@ -12841,7 +12744,7 @@
         <v>136527</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="22" t="s">
         <v>47</v>
       </c>
@@ -12895,7 +12798,7 @@
         <v>1668706</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="22" t="s">
         <v>49</v>
       </c>
@@ -12949,7 +12852,7 @@
         <v>10500375</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="22" t="s">
         <v>51</v>
       </c>
@@ -13003,7 +12906,7 @@
         <v>589946</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="22" t="s">
         <v>53</v>
       </c>

</xml_diff>